<commit_message>
Updated interstate demand code
</commit_message>
<xml_diff>
--- a/Multi Nodal Model/Interstate Data/Demand/Mapping Tables.xlsx
+++ b/Multi Nodal Model/Interstate Data/Demand/Mapping Tables.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harrison\Documents\Uni\Honours\ElectraNetHonours\Multi Nodal\Interstate Data\Demand Traces\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harrison\Documents\MILES-SA\Multi Nodal Model\Interstate Data\Demand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C343967C-1F75-41C5-B997-9825BCE6DEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8249F45-5259-40FA-87EC-439536FBB656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NSW Demand Files" sheetId="1" r:id="rId1"/>
     <sheet name="VIC Demand Files" sheetId="4" r:id="rId2"/>
-    <sheet name="Hydrogen Production" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,18 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>File Name</t>
   </si>
   <si>
     <t>Node Name</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>NSW</t>
   </si>
   <si>
     <t>VIC</t>
@@ -134,16 +127,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,9 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
@@ -443,43 +428,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -502,19 +487,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -528,207 +513,6 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71E2CA0-DDEF-47E7-82FC-02B491A08917}">
-  <dimension ref="A1:AC3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="16384" width="9.15234375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="4">
-        <v>2025</v>
-      </c>
-      <c r="C1" s="4">
-        <v>2026</v>
-      </c>
-      <c r="D1" s="4">
-        <v>2027</v>
-      </c>
-      <c r="E1" s="4">
-        <v>2028</v>
-      </c>
-      <c r="F1" s="4">
-        <v>2029</v>
-      </c>
-      <c r="G1" s="4">
-        <v>2030</v>
-      </c>
-      <c r="H1" s="4">
-        <v>2031</v>
-      </c>
-      <c r="I1" s="4">
-        <v>2032</v>
-      </c>
-      <c r="J1" s="4">
-        <v>2033</v>
-      </c>
-      <c r="K1" s="4">
-        <v>2034</v>
-      </c>
-      <c r="L1" s="4">
-        <v>2035</v>
-      </c>
-      <c r="M1" s="4">
-        <v>2036</v>
-      </c>
-      <c r="N1" s="4">
-        <v>2037</v>
-      </c>
-      <c r="O1" s="4">
-        <v>2038</v>
-      </c>
-      <c r="P1" s="4">
-        <v>2039</v>
-      </c>
-      <c r="Q1" s="4">
-        <v>2040</v>
-      </c>
-      <c r="R1" s="4">
-        <v>2041</v>
-      </c>
-      <c r="S1" s="4">
-        <v>2042</v>
-      </c>
-      <c r="T1" s="4">
-        <v>2043</v>
-      </c>
-      <c r="U1" s="4">
-        <v>2044</v>
-      </c>
-      <c r="V1" s="4">
-        <v>2045</v>
-      </c>
-      <c r="W1" s="4">
-        <v>2046</v>
-      </c>
-      <c r="X1" s="4">
-        <v>2047</v>
-      </c>
-      <c r="Y1" s="4">
-        <v>2048</v>
-      </c>
-      <c r="Z1" s="4">
-        <v>2049</v>
-      </c>
-      <c r="AA1" s="4">
-        <v>2050</v>
-      </c>
-      <c r="AB1" s="4">
-        <v>2051</v>
-      </c>
-      <c r="AC1" s="4">
-        <v>2052</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>8.8999999999999999E-3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.3977</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1.1494</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1.5476000000000001</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1.8864999999999998</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2.3157000000000001</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3.0543</v>
-      </c>
-      <c r="I2" s="1">
-        <v>3.1743000000000001</v>
-      </c>
-      <c r="J2" s="1">
-        <v>3.1438000000000001</v>
-      </c>
-      <c r="K2" s="1">
-        <v>3.5366</v>
-      </c>
-      <c r="L2" s="1">
-        <v>2.7470999999999997</v>
-      </c>
-      <c r="M2" s="1">
-        <v>2.9984000000000002</v>
-      </c>
-      <c r="N2" s="1">
-        <v>3.2793999999999999</v>
-      </c>
-      <c r="O2" s="1">
-        <v>3.7923</v>
-      </c>
-      <c r="P2" s="1">
-        <v>3.6083999999999996</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>3.9059999999999997</v>
-      </c>
-      <c r="R2" s="1">
-        <v>3.8812000000000002</v>
-      </c>
-      <c r="S2" s="1">
-        <v>4.8239000000000001</v>
-      </c>
-      <c r="T2" s="1">
-        <v>4.5663</v>
-      </c>
-      <c r="U2" s="1">
-        <v>4.8593000000000002</v>
-      </c>
-      <c r="V2" s="1">
-        <v>5.0010000000000003</v>
-      </c>
-      <c r="W2" s="1">
-        <v>4.7751999999999999</v>
-      </c>
-      <c r="X2" s="1">
-        <v>4.8319000000000001</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>4.8571</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>5.5471000000000004</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>5.5745000000000005</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>5.6908000000000003</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>5.8267000000000007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>